<commit_message>
fetcher makes csv file
</commit_message>
<xml_diff>
--- a/data-fetching/template.xlsx
+++ b/data-fetching/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff\Documents\Kuleuven\FeedbackVisuals\FeedbackVisuals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff\Documents\Kuleuven\FeedbackVisuals\FeedbackVisuals\data-fetching\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6662CC2-F500-4339-911A-15C596784B62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928AED49-EC76-47D5-9648-04BF68D4D7FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ECCF5C31-E73D-41E6-A20B-1B020134CB8E}"/>
   </bookViews>
@@ -33,15 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Questions</t>
   </si>
   <si>
     <t>Q4</t>
-  </si>
-  <si>
-    <t>totale score</t>
   </si>
   <si>
     <t>Q6</t>
@@ -70,6 +67,12 @@
   <si>
     <t>thema ('plan van aanpak' = 0;
 'Concepten '= 1; Wiskundig model = 2; Rekentechnische aanpak = 3; Fysische interpretatie = 4; Eigen aandachtspunt</t>
+  </si>
+  <si>
+    <t>soort vraag (multiple = 0, één aantwoord mogeljk = 1)</t>
+  </si>
+  <si>
+    <t>maximale score</t>
   </si>
 </sst>
 </file>
@@ -431,55 +434,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8FD038-3A68-48E2-8948-48864369A52F}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" customWidth="1"/>
     <col min="2" max="2" width="39.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>1</v>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="E1" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G1" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I1" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J1" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K1" s="1">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -487,268 +494,295 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>6</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>7</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>7</v>
       </c>
       <c r="E4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>6</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-      <c r="E8">
-        <v>6</v>
-      </c>
-      <c r="F8">
-        <v>5</v>
-      </c>
-      <c r="G8">
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <v>3</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="C10">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
         <v>1</v>
       </c>
     </row>

</xml_diff>